<commit_message>
Documentation and benchmark results
</commit_message>
<xml_diff>
--- a/map_testing/benchmark.xlsx
+++ b/map_testing/benchmark.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theif519\Documents\GitHub\go\map_testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\go\map_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7515" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20496" windowHeight="7512" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="intset" sheetId="1" r:id="rId1"/>
     <sheet name="combinedFile" sheetId="3" r:id="rId2"/>
-    <sheet name="iteratorRWFile" sheetId="4" r:id="rId3"/>
-    <sheet name="iteratorROFile" sheetId="2" r:id="rId4"/>
+    <sheet name="combinedFileSkim" sheetId="5" r:id="rId3"/>
+    <sheet name="iteratorRWFile" sheetId="4" r:id="rId4"/>
+    <sheet name="iteratorROFile" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Map-Intset</t>
   </si>
@@ -64,6 +65,15 @@
   </si>
   <si>
     <t>DefaultMap (No Lock)</t>
+  </si>
+  <si>
+    <t>Map-CombinedSkim</t>
+  </si>
+  <si>
+    <t>SynchronizedMap</t>
+  </si>
+  <si>
+    <t>ReaderWriterMap</t>
   </si>
 </sst>
 </file>
@@ -760,22 +770,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.24</c:v>
+                  <c:v>6.29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.54</c:v>
+                  <c:v>12.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.9</c:v>
+                  <c:v>27.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.22</c:v>
+                  <c:v>43.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.23</c:v>
+                  <c:v>41.67</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.22</c:v>
+                  <c:v>41.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -860,22 +870,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.13</c:v>
+                  <c:v>6.33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.72</c:v>
+                  <c:v>5.81</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.24</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.75</c:v>
+                  <c:v>4.13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.95</c:v>
+                  <c:v>4.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.85</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,22 +968,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.29</c:v>
+                  <c:v>6.33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.14</c:v>
+                  <c:v>3.21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.35</c:v>
+                  <c:v>3.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4700000000000002</c:v>
+                  <c:v>3.94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.98</c:v>
+                  <c:v>3.39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.17</c:v>
+                  <c:v>3.37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -986,7 +996,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1595,22 +1604,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.85</c:v>
+                  <c:v>21.74</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.87</c:v>
+                  <c:v>35.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.83</c:v>
+                  <c:v>71.430000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.48</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.56</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58.82</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1695,22 +1704,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.58</c:v>
+                  <c:v>23.81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.87</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.78</c:v>
+                  <c:v>76.92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47.62</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.56</c:v>
+                  <c:v>111.11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.5</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1793,22 +1802,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.7100000000000009</c:v>
+                  <c:v>38.46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.76</c:v>
+                  <c:v>35.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.99</c:v>
+                  <c:v>35.71</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.239999999999998</c:v>
+                  <c:v>35.71</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.29</c:v>
+                  <c:v>35.71</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.7</c:v>
+                  <c:v>35.71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1891,22 +1900,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10.42</c:v>
+                  <c:v>38.46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.1</c:v>
+                  <c:v>35.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6199999999999992</c:v>
+                  <c:v>37.04</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.42</c:v>
+                  <c:v>37.04</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.99</c:v>
+                  <c:v>37.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.53</c:v>
+                  <c:v>37.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1919,7 +1928,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2415,6 +2423,833 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Combined Skim</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - 2.5% Iteration (8-Core)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>combinedFileSkim!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ConcurrentMap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>combinedFileSkim!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>combinedFileSkim!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>22.22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-997E-4188-8571-5CBD24C3FA96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>combinedFileSkim!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ConcurrentMap-Interlocked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>combinedFileSkim!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>combinedFileSkim!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>23.26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>111.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-997E-4188-8571-5CBD24C3FA96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>combinedFileSkim!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SynchronizedMap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>combinedFileSkim!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>combinedFileSkim!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>38.46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-997E-4188-8571-5CBD24C3FA96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>combinedFileSkim!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ReaderWriterMap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>combinedFileSkim!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>combinedFileSkim!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>37.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-997E-4188-8571-5CBD24C3FA96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="217398872"/>
+        <c:axId val="217399200"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="217398872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Goroutines</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="217399200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="217399200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Million Ops/Sec</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="217398872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Microbenchmark</a:t>
             </a:r>
             <a:r>
@@ -2533,22 +3368,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.6</c:v>
+                  <c:v>5.41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4900000000000002</c:v>
+                  <c:v>5.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.21</c:v>
+                  <c:v>4.74</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.56</c:v>
+                  <c:v>2.84</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81</c:v>
+                  <c:v>1.67</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.41</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2633,22 +3468,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.26</c:v>
+                  <c:v>6.37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.33</c:v>
+                  <c:v>5.88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.16</c:v>
+                  <c:v>5.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.59</c:v>
+                  <c:v>3.91</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.82</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.47</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2731,22 +3566,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>20.41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.13</c:v>
+                  <c:v>9.6199999999999992</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4500000000000002</c:v>
+                  <c:v>4.6500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1499999999999999</c:v>
+                  <c:v>2.33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>1.1599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.33</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2829,22 +3664,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10.1</c:v>
+                  <c:v>19.61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.65</c:v>
+                  <c:v>9.6199999999999992</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.77</c:v>
+                  <c:v>4.67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.38</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.68</c:v>
+                  <c:v>1.1499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2857,7 +3692,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3335,7 +4169,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3487,22 +4321,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>15.87</c:v>
+                  <c:v>37.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.7</c:v>
+                  <c:v>32.26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.08</c:v>
+                  <c:v>28.57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.05</c:v>
+                  <c:v>20.83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.79</c:v>
+                  <c:v>10.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4500000000000002</c:v>
+                  <c:v>5.29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3587,22 +4421,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>17.86</c:v>
+                  <c:v>43.48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.62</c:v>
+                  <c:v>33.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.38</c:v>
+                  <c:v>32.26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.81</c:v>
+                  <c:v>22.22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.85</c:v>
+                  <c:v>10.31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2799999999999998</c:v>
+                  <c:v>5.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3685,22 +4519,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>33.33</c:v>
+                  <c:v>66.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.57</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.26</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.76</c:v>
+                  <c:v>35.71</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.52</c:v>
+                  <c:v>17.86</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.97</c:v>
+                  <c:v>9.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3713,7 +4547,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4352,6 +5185,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
@@ -5916,6 +6789,527 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6514,6 +7908,41 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
@@ -6543,20 +7972,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:rowOff>4760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>129539</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6877,13 +8306,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6906,73 +8335,73 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4.24</v>
+        <v>6.29</v>
       </c>
       <c r="C2">
-        <v>6.54</v>
+        <v>12.66</v>
       </c>
       <c r="D2">
-        <v>11.9</v>
+        <v>27.03</v>
       </c>
       <c r="E2">
-        <v>22.22</v>
+        <v>43.48</v>
       </c>
       <c r="F2">
-        <v>19.23</v>
+        <v>41.67</v>
       </c>
       <c r="G2">
-        <v>22.22</v>
+        <v>41.67</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>5.13</v>
+        <v>6.33</v>
       </c>
       <c r="C3">
-        <v>3.72</v>
+        <v>5.81</v>
       </c>
       <c r="D3">
-        <v>3.24</v>
+        <v>4.5</v>
       </c>
       <c r="E3">
-        <v>2.75</v>
+        <v>4.13</v>
       </c>
       <c r="F3">
-        <v>2.95</v>
+        <v>4.03</v>
       </c>
       <c r="G3">
-        <v>2.85</v>
+        <v>4.2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4">
-        <v>4.29</v>
+        <v>6.33</v>
       </c>
       <c r="C4">
-        <v>2.14</v>
+        <v>3.21</v>
       </c>
       <c r="D4">
-        <v>2.35</v>
+        <v>3.64</v>
       </c>
       <c r="E4">
-        <v>2.4700000000000002</v>
+        <v>3.94</v>
       </c>
       <c r="F4">
-        <v>1.98</v>
+        <v>3.39</v>
       </c>
       <c r="G4">
-        <v>2.17</v>
+        <v>3.37</v>
       </c>
     </row>
   </sheetData>
@@ -6985,13 +8414,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -7014,96 +8443,96 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>6.85</v>
+        <v>21.74</v>
       </c>
       <c r="C2">
-        <v>10.87</v>
+        <v>35.71</v>
       </c>
       <c r="D2">
-        <v>20.83</v>
+        <v>71.430000000000007</v>
       </c>
       <c r="E2">
-        <v>43.48</v>
+        <v>100</v>
       </c>
       <c r="F2">
-        <v>55.56</v>
+        <v>100</v>
       </c>
       <c r="G2">
-        <v>58.82</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>6.58</v>
+        <v>23.81</v>
       </c>
       <c r="C3">
-        <v>10.87</v>
+        <v>40</v>
       </c>
       <c r="D3">
-        <v>27.78</v>
+        <v>76.92</v>
       </c>
       <c r="E3">
-        <v>47.62</v>
+        <v>100</v>
       </c>
       <c r="F3">
-        <v>55.56</v>
+        <v>111.11</v>
       </c>
       <c r="G3">
-        <v>62.5</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4">
-        <v>9.7100000000000009</v>
+        <v>38.46</v>
       </c>
       <c r="C4">
-        <v>11.76</v>
+        <v>35.71</v>
       </c>
       <c r="D4">
-        <v>12.99</v>
+        <v>35.71</v>
       </c>
       <c r="E4">
-        <v>17.239999999999998</v>
+        <v>35.71</v>
       </c>
       <c r="F4">
-        <v>14.29</v>
+        <v>35.71</v>
       </c>
       <c r="G4">
-        <v>13.7</v>
+        <v>35.71</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
-        <v>10.42</v>
+        <v>38.46</v>
       </c>
       <c r="C5">
-        <v>10.1</v>
+        <v>35.71</v>
       </c>
       <c r="D5">
-        <v>9.6199999999999992</v>
+        <v>37.04</v>
       </c>
       <c r="E5">
-        <v>10.42</v>
+        <v>37.04</v>
       </c>
       <c r="F5">
-        <v>10.99</v>
+        <v>37.04</v>
       </c>
       <c r="G5">
-        <v>10.53</v>
+        <v>37.04</v>
       </c>
     </row>
   </sheetData>
@@ -7114,17 +8543,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -7145,119 +8574,96 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2.6</v>
+        <v>22.22</v>
       </c>
       <c r="C2">
-        <v>2.4900000000000002</v>
+        <v>38.46</v>
       </c>
       <c r="D2">
-        <v>2.21</v>
+        <v>66.67</v>
       </c>
       <c r="E2">
-        <v>1.56</v>
+        <v>100</v>
       </c>
       <c r="F2">
-        <v>0.81</v>
+        <v>100</v>
       </c>
       <c r="G2">
-        <v>0.41</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3.26</v>
+        <v>23.26</v>
       </c>
       <c r="C3">
-        <v>2.33</v>
+        <v>38.46</v>
       </c>
       <c r="D3">
-        <v>2.16</v>
+        <v>66.67</v>
       </c>
       <c r="E3">
-        <v>1.59</v>
+        <v>90.91</v>
       </c>
       <c r="F3">
-        <v>0.82</v>
+        <v>100</v>
       </c>
       <c r="G3">
-        <v>0.47</v>
+        <v>111.11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>38.46</v>
       </c>
       <c r="C4">
-        <v>4.13</v>
+        <v>33.33</v>
       </c>
       <c r="D4">
-        <v>2.4500000000000002</v>
+        <v>32.26</v>
       </c>
       <c r="E4">
-        <v>1.1499999999999999</v>
+        <v>32.26</v>
       </c>
       <c r="F4">
-        <v>0.55000000000000004</v>
+        <v>32.26</v>
       </c>
       <c r="G4">
-        <v>0.33</v>
+        <v>32.26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>10.1</v>
+        <v>37.04</v>
       </c>
       <c r="C5">
-        <v>5.65</v>
+        <v>32.26</v>
       </c>
       <c r="D5">
-        <v>2.77</v>
+        <v>32.26</v>
       </c>
       <c r="E5">
-        <v>1.38</v>
+        <v>32.26</v>
       </c>
       <c r="F5">
-        <v>0.68</v>
+        <v>32.26</v>
       </c>
       <c r="G5">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>3.39</v>
-      </c>
-      <c r="C6">
-        <v>1.3</v>
-      </c>
-      <c r="D6">
-        <v>0.45</v>
-      </c>
-      <c r="E6">
-        <v>0.2</v>
-      </c>
-      <c r="F6">
-        <v>0.09</v>
-      </c>
-      <c r="G6">
-        <v>0.05</v>
+        <v>32.26</v>
       </c>
     </row>
   </sheetData>
@@ -7268,15 +8674,169 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>16</v>
+      </c>
+      <c r="G1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5.41</v>
+      </c>
+      <c r="C2">
+        <v>5.08</v>
+      </c>
+      <c r="D2">
+        <v>4.74</v>
+      </c>
+      <c r="E2">
+        <v>2.84</v>
+      </c>
+      <c r="F2">
+        <v>1.67</v>
+      </c>
+      <c r="G2">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6.37</v>
+      </c>
+      <c r="C3">
+        <v>5.88</v>
+      </c>
+      <c r="D3">
+        <v>5.52</v>
+      </c>
+      <c r="E3">
+        <v>3.91</v>
+      </c>
+      <c r="F3">
+        <v>1.9</v>
+      </c>
+      <c r="G3">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>20.41</v>
+      </c>
+      <c r="C4">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="D4">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="E4">
+        <v>2.33</v>
+      </c>
+      <c r="F4">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G4">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>19.61</v>
+      </c>
+      <c r="C5">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="D5">
+        <v>4.67</v>
+      </c>
+      <c r="E5">
+        <v>2.25</v>
+      </c>
+      <c r="F5">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3.39</v>
+      </c>
+      <c r="C6">
+        <v>1.3</v>
+      </c>
+      <c r="D6">
+        <v>0.45</v>
+      </c>
+      <c r="E6">
+        <v>0.2</v>
+      </c>
+      <c r="F6">
+        <v>0.09</v>
+      </c>
+      <c r="G6">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -7299,73 +8859,73 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>15.87</v>
+        <v>37.04</v>
       </c>
       <c r="C2">
-        <v>13.7</v>
+        <v>32.26</v>
       </c>
       <c r="D2">
-        <v>14.08</v>
+        <v>28.57</v>
       </c>
       <c r="E2">
-        <v>5.05</v>
+        <v>20.83</v>
       </c>
       <c r="F2">
-        <v>3.79</v>
+        <v>10.42</v>
       </c>
       <c r="G2">
-        <v>2.4500000000000002</v>
+        <v>5.29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>17.86</v>
+        <v>43.48</v>
       </c>
       <c r="C3">
-        <v>15.62</v>
+        <v>33.33</v>
       </c>
       <c r="D3">
-        <v>15.38</v>
+        <v>32.26</v>
       </c>
       <c r="E3">
-        <v>7.81</v>
+        <v>22.22</v>
       </c>
       <c r="F3">
-        <v>3.85</v>
+        <v>10.31</v>
       </c>
       <c r="G3">
-        <v>2.2799999999999998</v>
+        <v>5.08</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4">
-        <v>33.33</v>
+        <v>66.67</v>
       </c>
       <c r="C4">
-        <v>28.57</v>
+        <v>62.5</v>
       </c>
       <c r="D4">
-        <v>23.26</v>
+        <v>62.5</v>
       </c>
       <c r="E4">
-        <v>11.76</v>
+        <v>35.71</v>
       </c>
       <c r="F4">
-        <v>7.52</v>
+        <v>17.86</v>
       </c>
       <c r="G4">
-        <v>3.97</v>
+        <v>9.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) Added instrumentation for sync.Interlocked scoped map functions. They now access a faster cached version of their respective functions. This shows sync.Interlocked to be magnitudes faster for read-modify-write operations during iteration
2) Sync.Interlocked blocks now support deletion while iterating. Needs
to be further tested...

3) Sync.Interlocked iteration now has a race condition (scary thing
is... did it ever truly work? I'll find out soon) during iteration. Need
to fix, not sure of cause.

4) While Read-Write iteration performance has skyrocketed, the
performance of all other functions seem to have decreased? Looking into
that.
</commit_message>
<xml_diff>
--- a/map_testing/benchmark.xlsx
+++ b/map_testing/benchmark.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Map-Intset</t>
   </si>
@@ -44,18 +44,6 @@
   </si>
   <si>
     <t>Map-IteratorRW</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>SynchronizedMap (Mutex)</t>
@@ -770,22 +758,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.29</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.66</c:v>
+                  <c:v>7.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.03</c:v>
+                  <c:v>13.33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.48</c:v>
+                  <c:v>20.83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.67</c:v>
+                  <c:v>21.74</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.67</c:v>
+                  <c:v>21.28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -870,22 +858,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.33</c:v>
+                  <c:v>6.21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.81</c:v>
+                  <c:v>5.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5</c:v>
+                  <c:v>4.4800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.13</c:v>
+                  <c:v>4.07</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.03</c:v>
+                  <c:v>4.12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2</c:v>
+                  <c:v>4.1500000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -971,19 +959,19 @@
                   <c:v>6.33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.21</c:v>
+                  <c:v>3.91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.64</c:v>
+                  <c:v>3.53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.94</c:v>
+                  <c:v>3.55</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.39</c:v>
+                  <c:v>2.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.37</c:v>
+                  <c:v>3.29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1604,19 +1592,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>21.74</c:v>
+                  <c:v>21.28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.71</c:v>
+                  <c:v>34.479999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.430000000000007</c:v>
+                  <c:v>66.67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>90.91</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>90.91</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100</c:v>
@@ -1704,22 +1692,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>23.81</c:v>
+                  <c:v>19.23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>33.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>76.92</c:v>
+                  <c:v>58.82</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>83.33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>111.11</c:v>
+                  <c:v>83.33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>83.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1802,22 +1790,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>38.46</c:v>
+                  <c:v>32.26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.71</c:v>
+                  <c:v>27.78</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.71</c:v>
+                  <c:v>27.78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.71</c:v>
+                  <c:v>27.78</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.71</c:v>
+                  <c:v>27.78</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.71</c:v>
+                  <c:v>27.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1900,22 +1888,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>38.46</c:v>
+                  <c:v>30.26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.71</c:v>
+                  <c:v>25.78</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.04</c:v>
+                  <c:v>25.78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.04</c:v>
+                  <c:v>25.78</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.04</c:v>
+                  <c:v>25.78</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.04</c:v>
+                  <c:v>25.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2427,7 +2415,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> - 2.5% Iteration (8-Core)</a:t>
+              <a:t> - 2.5% Read-Write Iteration (8-Core)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2541,22 +2529,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>22.22</c:v>
+                  <c:v>1.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.46</c:v>
+                  <c:v>3.21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66.67</c:v>
+                  <c:v>6.17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>8.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>7.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2641,22 +2629,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>23.26</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.46</c:v>
+                  <c:v>18.87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66.67</c:v>
+                  <c:v>29.41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.91</c:v>
+                  <c:v>45.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>45.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>111.11</c:v>
+                  <c:v>47.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2739,22 +2727,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>38.46</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.33</c:v>
+                  <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.26</c:v>
+                  <c:v>11.63</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.26</c:v>
+                  <c:v>11.76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.26</c:v>
+                  <c:v>11.63</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.26</c:v>
+                  <c:v>11.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2837,22 +2825,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>37.04</c:v>
+                  <c:v>12.35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.26</c:v>
+                  <c:v>11.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.26</c:v>
+                  <c:v>11.49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.26</c:v>
+                  <c:v>11.76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.26</c:v>
+                  <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.26</c:v>
+                  <c:v>11.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2865,7 +2853,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3368,22 +3355,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.41</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.08</c:v>
+                  <c:v>1.99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.74</c:v>
+                  <c:v>1.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.84</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.67</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.82</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3468,22 +3455,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.37</c:v>
+                  <c:v>16.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.88</c:v>
+                  <c:v>13.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.52</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.91</c:v>
+                  <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9</c:v>
+                  <c:v>4.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.96</c:v>
+                  <c:v>2.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3566,22 +3553,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>20.41</c:v>
+                  <c:v>16.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6199999999999992</c:v>
+                  <c:v>8.93</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6500000000000004</c:v>
+                  <c:v>4.29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.33</c:v>
+                  <c:v>2.17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1599999999999999</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3664,22 +3651,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>19.61</c:v>
+                  <c:v>18.87</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6199999999999992</c:v>
+                  <c:v>8.93</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.67</c:v>
+                  <c:v>4.3899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.25</c:v>
+                  <c:v>2.16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1499999999999999</c:v>
+                  <c:v>1.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4321,22 +4308,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>37.04</c:v>
+                  <c:v>33.33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.26</c:v>
+                  <c:v>30.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.57</c:v>
+                  <c:v>25.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.83</c:v>
+                  <c:v>18.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.42</c:v>
+                  <c:v>9.09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.29</c:v>
+                  <c:v>4.63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4421,22 +4408,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>43.48</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.33</c:v>
+                  <c:v>26.32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.26</c:v>
+                  <c:v>24.39</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.22</c:v>
+                  <c:v>18.18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.31</c:v>
+                  <c:v>8.5500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.08</c:v>
+                  <c:v>4.26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4519,22 +4506,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>66.67</c:v>
+                  <c:v>58.82</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.5</c:v>
+                  <c:v>55.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.5</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.71</c:v>
+                  <c:v>32.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.86</c:v>
+                  <c:v>15.87</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.01</c:v>
+                  <c:v>7.87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8306,8 +8293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8340,68 +8327,68 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>6.29</v>
+        <v>3.7</v>
       </c>
       <c r="C2">
-        <v>12.66</v>
+        <v>7.19</v>
       </c>
       <c r="D2">
-        <v>27.03</v>
+        <v>13.33</v>
       </c>
       <c r="E2">
-        <v>43.48</v>
+        <v>20.83</v>
       </c>
       <c r="F2">
-        <v>41.67</v>
+        <v>21.74</v>
       </c>
       <c r="G2">
-        <v>41.67</v>
+        <v>21.28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>6.33</v>
+        <v>6.21</v>
       </c>
       <c r="C3">
-        <v>5.81</v>
+        <v>5.71</v>
       </c>
       <c r="D3">
-        <v>4.5</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="E3">
-        <v>4.13</v>
+        <v>4.07</v>
       </c>
       <c r="F3">
-        <v>4.03</v>
+        <v>4.12</v>
       </c>
       <c r="G3">
-        <v>4.2</v>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>6.33</v>
       </c>
       <c r="C4">
-        <v>3.21</v>
+        <v>3.91</v>
       </c>
       <c r="D4">
-        <v>3.64</v>
+        <v>3.53</v>
       </c>
       <c r="E4">
-        <v>3.94</v>
+        <v>3.55</v>
       </c>
       <c r="F4">
-        <v>3.39</v>
+        <v>2.82</v>
       </c>
       <c r="G4">
-        <v>3.37</v>
+        <v>3.29</v>
       </c>
     </row>
   </sheetData>
@@ -8414,8 +8401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8448,19 +8435,19 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>21.74</v>
+        <v>21.28</v>
       </c>
       <c r="C2">
-        <v>35.71</v>
+        <v>34.479999999999997</v>
       </c>
       <c r="D2">
-        <v>71.430000000000007</v>
+        <v>66.67</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>90.91</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>90.91</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -8471,68 +8458,68 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>23.81</v>
+        <v>19.23</v>
       </c>
       <c r="C3">
-        <v>40</v>
+        <v>33.33</v>
       </c>
       <c r="D3">
-        <v>76.92</v>
+        <v>58.82</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>83.33</v>
       </c>
       <c r="F3">
-        <v>111.11</v>
+        <v>83.33</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>83.33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>38.46</v>
+        <v>32.26</v>
       </c>
       <c r="C4">
-        <v>35.71</v>
+        <v>27.78</v>
       </c>
       <c r="D4">
-        <v>35.71</v>
+        <v>27.78</v>
       </c>
       <c r="E4">
-        <v>35.71</v>
+        <v>27.78</v>
       </c>
       <c r="F4">
-        <v>35.71</v>
+        <v>27.78</v>
       </c>
       <c r="G4">
-        <v>35.71</v>
+        <v>27.78</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>38.46</v>
+        <v>30.26</v>
       </c>
       <c r="C5">
-        <v>35.71</v>
+        <v>25.78</v>
       </c>
       <c r="D5">
-        <v>37.04</v>
+        <v>25.78</v>
       </c>
       <c r="E5">
-        <v>37.04</v>
+        <v>25.78</v>
       </c>
       <c r="F5">
-        <v>37.04</v>
+        <v>25.78</v>
       </c>
       <c r="G5">
-        <v>37.04</v>
+        <v>25.78</v>
       </c>
     </row>
   </sheetData>
@@ -8553,7 +8540,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -8579,22 +8566,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>22.22</v>
+        <v>1.92</v>
       </c>
       <c r="C2">
-        <v>38.46</v>
+        <v>3.21</v>
       </c>
       <c r="D2">
-        <v>66.67</v>
+        <v>6.17</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>8.06</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>7.94</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -8602,68 +8589,68 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>23.26</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C3">
-        <v>38.46</v>
+        <v>18.87</v>
       </c>
       <c r="D3">
-        <v>66.67</v>
+        <v>29.41</v>
       </c>
       <c r="E3">
-        <v>90.91</v>
+        <v>45.45</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>45.45</v>
       </c>
       <c r="G3">
-        <v>111.11</v>
+        <v>47.62</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>38.46</v>
+        <v>12.2</v>
       </c>
       <c r="C4">
-        <v>33.33</v>
+        <v>11.9</v>
       </c>
       <c r="D4">
-        <v>32.26</v>
+        <v>11.63</v>
       </c>
       <c r="E4">
-        <v>32.26</v>
+        <v>11.76</v>
       </c>
       <c r="F4">
-        <v>32.26</v>
+        <v>11.63</v>
       </c>
       <c r="G4">
-        <v>32.26</v>
+        <v>11.76</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>37.04</v>
+        <v>12.35</v>
       </c>
       <c r="C5">
-        <v>32.26</v>
+        <v>11.76</v>
       </c>
       <c r="D5">
-        <v>32.26</v>
+        <v>11.49</v>
       </c>
       <c r="E5">
-        <v>32.26</v>
+        <v>11.76</v>
       </c>
       <c r="F5">
-        <v>32.26</v>
+        <v>11.9</v>
       </c>
       <c r="G5">
-        <v>32.26</v>
+        <v>11.9</v>
       </c>
     </row>
   </sheetData>
@@ -8677,7 +8664,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8710,22 +8697,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5.41</v>
+        <v>2.25</v>
       </c>
       <c r="C2">
-        <v>5.08</v>
+        <v>1.99</v>
       </c>
       <c r="D2">
-        <v>4.74</v>
+        <v>1.95</v>
       </c>
       <c r="E2">
-        <v>2.84</v>
+        <v>1.04</v>
       </c>
       <c r="F2">
-        <v>1.67</v>
+        <v>0.49</v>
       </c>
       <c r="G2">
-        <v>0.82</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -8733,68 +8720,68 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>6.37</v>
+        <v>16.39</v>
       </c>
       <c r="C3">
-        <v>5.88</v>
+        <v>13.89</v>
       </c>
       <c r="D3">
-        <v>5.52</v>
+        <v>12.5</v>
       </c>
       <c r="E3">
-        <v>3.91</v>
+        <v>8.4</v>
       </c>
       <c r="F3">
-        <v>1.9</v>
+        <v>4.22</v>
       </c>
       <c r="G3">
-        <v>0.96</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>20.41</v>
+        <v>16.39</v>
       </c>
       <c r="C4">
-        <v>9.6199999999999992</v>
+        <v>8.93</v>
       </c>
       <c r="D4">
-        <v>4.6500000000000004</v>
+        <v>4.29</v>
       </c>
       <c r="E4">
-        <v>2.33</v>
+        <v>2.17</v>
       </c>
       <c r="F4">
-        <v>1.1599999999999999</v>
+        <v>1.04</v>
       </c>
       <c r="G4">
-        <v>0.57999999999999996</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>19.61</v>
+        <v>18.87</v>
       </c>
       <c r="C5">
-        <v>9.6199999999999992</v>
+        <v>8.93</v>
       </c>
       <c r="D5">
-        <v>4.67</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="E5">
-        <v>2.25</v>
+        <v>2.16</v>
       </c>
       <c r="F5">
-        <v>1.1499999999999999</v>
+        <v>1.06</v>
       </c>
       <c r="G5">
-        <v>0.56999999999999995</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -8831,7 +8818,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8864,22 +8851,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>37.04</v>
+        <v>33.33</v>
       </c>
       <c r="C2">
-        <v>32.26</v>
+        <v>30.3</v>
       </c>
       <c r="D2">
-        <v>28.57</v>
+        <v>25.64</v>
       </c>
       <c r="E2">
-        <v>20.83</v>
+        <v>18.52</v>
       </c>
       <c r="F2">
-        <v>10.42</v>
+        <v>9.09</v>
       </c>
       <c r="G2">
-        <v>5.29</v>
+        <v>4.63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -8887,45 +8874,45 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>43.48</v>
+        <v>31.25</v>
       </c>
       <c r="C3">
-        <v>33.33</v>
+        <v>26.32</v>
       </c>
       <c r="D3">
-        <v>32.26</v>
+        <v>24.39</v>
       </c>
       <c r="E3">
-        <v>22.22</v>
+        <v>18.18</v>
       </c>
       <c r="F3">
-        <v>10.31</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="G3">
-        <v>5.08</v>
+        <v>4.26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>66.67</v>
+        <v>58.82</v>
       </c>
       <c r="C4">
-        <v>62.5</v>
+        <v>55.56</v>
       </c>
       <c r="D4">
-        <v>62.5</v>
+        <v>50</v>
       </c>
       <c r="E4">
-        <v>35.71</v>
+        <v>32.26</v>
       </c>
       <c r="F4">
-        <v>17.86</v>
+        <v>15.87</v>
       </c>
       <c r="G4">
-        <v>9.01</v>
+        <v>7.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished removing sync.Interlocked keyword entirely. Iteration by default is now interlocked, and the interlocked region has been replaced for sync.Interlocked function which accepts a closure instead for it's body. Is it pretty? No. Oh well though.
</commit_message>
<xml_diff>
--- a/map_testing/benchmark.xlsx
+++ b/map_testing/benchmark.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -23,15 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Map-Intset</t>
   </si>
   <si>
     <t>ConcurrentMap</t>
-  </si>
-  <si>
-    <t>ConcurrentMap-Interlocked</t>
   </si>
   <si>
     <t>Map-IteratorRO</t>
@@ -56,9 +53,6 @@
   </si>
   <si>
     <t>ReaderWriterMap</t>
-  </si>
-  <si>
-    <t>ConcurrentMap (Interlocked)</t>
   </si>
   <si>
     <t>DefaultMap (No Mutex)</t>
@@ -644,7 +638,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> (8-Core)</a:t>
+              <a:t> (24-Core)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -726,10 +720,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>intset!$B$1:$G$1</c:f>
+              <c:f>intset!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -740,12 +734,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -753,27 +768,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>intset!$B$2:$G$2</c:f>
+              <c:f>intset!$B$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>3.7</c:v>
+                  <c:v>2.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.19</c:v>
+                  <c:v>4.8499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.33</c:v>
+                  <c:v>8.4700000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.83</c:v>
+                  <c:v>11.76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.74</c:v>
+                  <c:v>13.89</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.28</c:v>
+                  <c:v>16.13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.61</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.64</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -826,10 +862,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>intset!$B$1:$G$1</c:f>
+              <c:f>intset!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -840,12 +876,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -853,27 +910,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>intset!$B$3:$G$3</c:f>
+              <c:f>intset!$B$3:$N$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>6.21</c:v>
+                  <c:v>6.33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.71</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4800000000000004</c:v>
+                  <c:v>3.66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.07</c:v>
+                  <c:v>3.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.12</c:v>
+                  <c:v>2.86</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1500000000000004</c:v>
+                  <c:v>2.74</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.67</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2400000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -924,10 +1002,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>intset!$B$1:$G$1</c:f>
+              <c:f>intset!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -938,12 +1016,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -951,27 +1050,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>intset!$B$4:$G$4</c:f>
+              <c:f>intset!$B$4:$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>6.33</c:v>
+                  <c:v>5.71</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.91</c:v>
+                  <c:v>4.3099999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.53</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.55</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.82</c:v>
+                  <c:v>4.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.29</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.03</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1035,13 +1155,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>intset!$B$1:$G$1</c15:sqref>
+                          <c15:sqref>intset!$B$1:$N$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="13"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -1052,12 +1172,33 @@
                         <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="5">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
                         <c:v>16</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="9">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
                         <c:v>32</c:v>
                       </c:pt>
                     </c:numCache>
@@ -1085,13 +1226,13 @@
                         <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="4">
-                        <c:v>16</c:v>
-                      </c:pt>
                       <c:pt idx="5">
-                        <c:v>32</c:v>
+                        <c:v>10</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1479,7 +1620,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Microbenchmark - Combined (8-core)</a:t>
+              <a:t>Microbenchmark - Combined (24-core)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1520,8 +1661,8 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>combinedFile!$A$2</c:f>
@@ -1529,106 +1670,6 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>ConcurrentMap</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>combinedFile!$B$1:$G$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>combinedFile!$B$2:$G$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>21.28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>34.479999999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66.67</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>90.91</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90.91</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BE45-4C25-A0FE-13F21B9F3CEF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>combinedFile!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ConcurrentMap-Interlocked</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1660,10 +1701,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>combinedFile!$B$1:$G$1</c:f>
+              <c:f>combinedFile!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1674,12 +1715,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -1687,27 +1749,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>combinedFile!$B$3:$G$3</c:f>
+              <c:f>combinedFile!$B$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>19.23</c:v>
+                  <c:v>13.16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.33</c:v>
+                  <c:v>17.86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58.82</c:v>
+                  <c:v>35.71</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83.33</c:v>
+                  <c:v>55.56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83.33</c:v>
+                  <c:v>76.92</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83.33</c:v>
+                  <c:v>90.91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>111.11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>142.86000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>166.67</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>166.67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>166.67</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>166.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1724,7 +1807,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>combinedFile!$A$4</c:f>
+              <c:f>combinedFile!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1758,10 +1841,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>combinedFile!$B$1:$G$1</c:f>
+              <c:f>combinedFile!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1772,12 +1855,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -1785,27 +1889,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>combinedFile!$B$4:$G$4</c:f>
+              <c:f>combinedFile!$B$3:$N$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>32.26</c:v>
+                  <c:v>25.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.78</c:v>
+                  <c:v>23.81</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.78</c:v>
+                  <c:v>23.26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.78</c:v>
+                  <c:v>23.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.78</c:v>
+                  <c:v>23.26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.78</c:v>
+                  <c:v>23.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23.26</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23.26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1822,7 +1947,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>combinedFile!$A$5</c:f>
+              <c:f>combinedFile!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1856,10 +1981,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>combinedFile!$B$1:$G$1</c:f>
+              <c:f>combinedFile!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1870,12 +1995,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -1883,27 +2029,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>combinedFile!$B$5:$G$5</c:f>
+              <c:f>combinedFile!$B$4:$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>30.26</c:v>
+                  <c:v>25.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.78</c:v>
+                  <c:v>19.61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.78</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.78</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.78</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.78</c:v>
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1967,13 +2134,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>combinedFile!$B$1:$G$1</c15:sqref>
+                          <c15:sqref>combinedFile!$B$1:$N$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="13"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -1984,12 +2151,33 @@
                         <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="5">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
                         <c:v>16</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="9">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
                         <c:v>32</c:v>
                       </c:pt>
                     </c:numCache>
@@ -2017,13 +2205,13 @@
                         <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="4">
-                        <c:v>16</c:v>
-                      </c:pt>
                       <c:pt idx="5">
-                        <c:v>32</c:v>
+                        <c:v>10</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2032,6 +2220,132 @@
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-BE45-4C25-A0FE-13F21B9F3CEF}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>combinedFile!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="square"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>combinedFile!$B$1:$N$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>32</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>combinedFile!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-BE45-4C25-A0FE-13F21B9F3CEF}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -2415,7 +2729,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> - 2.5% Read-Write Iteration (8-Core)</a:t>
+              <a:t> - 2.5% Read-Write Iteration (24-Core)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2497,10 +2811,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>combinedFileSkim!$B$1:$G$1</c:f>
+              <c:f>combinedFileSkim!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2511,12 +2825,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -2524,27 +2859,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>combinedFileSkim!$B$2:$G$2</c:f>
+              <c:f>combinedFileSkim!$B$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.92</c:v>
+                  <c:v>7.35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.21</c:v>
+                  <c:v>10.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.17</c:v>
+                  <c:v>22.73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.1999999999999993</c:v>
+                  <c:v>34.479999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.06</c:v>
+                  <c:v>43.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.94</c:v>
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>71.430000000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>76.92</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90.91</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90.91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2557,111 +2913,11 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>combinedFileSkim!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ConcurrentMap-Interlocked</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>combinedFileSkim!$B$1:$G$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>combinedFileSkim!$B$3:$G$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.87</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>29.41</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45.45</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45.45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47.62</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-997E-4188-8571-5CBD24C3FA96}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="3"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>combinedFileSkim!$A$4</c:f>
+              <c:f>combinedFileSkim!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2695,10 +2951,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>combinedFileSkim!$B$1:$G$1</c:f>
+              <c:f>combinedFileSkim!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2709,12 +2965,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -2722,27 +2999,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>combinedFileSkim!$B$4:$G$4</c:f>
+              <c:f>combinedFileSkim!$B$3:$N$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>12.2</c:v>
+                  <c:v>8.5500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.9</c:v>
+                  <c:v>8.26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.63</c:v>
+                  <c:v>8.1300000000000008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.76</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.63</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.76</c:v>
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.26</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2759,7 +3057,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>combinedFileSkim!$A$5</c:f>
+              <c:f>combinedFileSkim!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2793,10 +3091,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>combinedFileSkim!$B$1:$G$1</c:f>
+              <c:f>combinedFileSkim!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2807,12 +3105,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -2820,27 +3139,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>combinedFileSkim!$B$5:$G$5</c:f>
+              <c:f>combinedFileSkim!$B$4:$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>12.35</c:v>
+                  <c:v>8.6199999999999992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.76</c:v>
+                  <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.49</c:v>
+                  <c:v>8.26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.76</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.9</c:v>
+                  <c:v>8.26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.9</c:v>
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.26</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2864,6 +3204,136 @@
         <c:smooth val="0"/>
         <c:axId val="217398872"/>
         <c:axId val="217399200"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>combinedFileSkim!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="triangle"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>combinedFileSkim!$B$1:$N$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>32</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>combinedFileSkim!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-997E-4188-8571-5CBD24C3FA96}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="217398872"/>
@@ -3241,7 +3711,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> - Read-Write Iteration (8-Core)</a:t>
+              <a:t> - Read-Write Iteration (24-Core)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3291,7 +3761,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ConcurrentMap (Interlocked)</c:v>
+                  <c:v>ConcurrentMap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3323,10 +3793,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>iteratorRWFile!$B$1:$G$1</c:f>
+              <c:f>iteratorRWFile!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3337,12 +3807,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -3350,27 +3841,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>iteratorRWFile!$B$2:$G$2</c:f>
+              <c:f>iteratorRWFile!$B$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>16.13</c:v>
+                  <c:v>11.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.78</c:v>
+                  <c:v>16.39</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>33.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>71.430000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>66.67</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>66.67</c:v>
+                  <c:v>83.33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>111.11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>111.11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>142.86000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3423,10 +3935,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>iteratorRWFile!$B$1:$G$1</c:f>
+              <c:f>iteratorRWFile!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3437,12 +3949,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -3450,27 +3983,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>iteratorRWFile!$B$3:$G$3</c:f>
+              <c:f>iteratorRWFile!$B$3:$N$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>18.52</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.86</c:v>
+                  <c:v>9.6199999999999992</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.54</c:v>
+                  <c:v>9.7100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.54</c:v>
+                  <c:v>9.7100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.54</c:v>
+                  <c:v>9.7100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.54</c:v>
+                  <c:v>9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.7100000000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3521,10 +4075,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>iteratorRWFile!$B$1:$G$1</c:f>
+              <c:f>iteratorRWFile!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3535,12 +4089,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -3548,27 +4123,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>iteratorRWFile!$B$4:$G$4</c:f>
+              <c:f>iteratorRWFile!$B$4:$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>18.52</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.54</c:v>
+                  <c:v>9.7100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.239999999999998</c:v>
+                  <c:v>9.6199999999999992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.239999999999998</c:v>
+                  <c:v>9.6199999999999992</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.239999999999998</c:v>
+                  <c:v>9.6199999999999992</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.239999999999998</c:v>
+                  <c:v>9.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.52</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.6199999999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3645,13 +4241,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>iteratorRWFile!$B$1:$G$1</c15:sqref>
+                          <c15:sqref>iteratorRWFile!$B$1:$N$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="13"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -3662,12 +4258,33 @@
                         <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="5">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
                         <c:v>16</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="9">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
                         <c:v>32</c:v>
                       </c:pt>
                     </c:numCache>
@@ -3695,13 +4312,13 @@
                         <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="4">
-                        <c:v>16</c:v>
-                      </c:pt>
                       <c:pt idx="5">
-                        <c:v>32</c:v>
+                        <c:v>10</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3720,7 +4337,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>iteratorRWFile!#REF!</c15:sqref>
@@ -3763,13 +4380,13 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>iteratorRWFile!$B$1:$G$1</c15:sqref>
+                          <c15:sqref>iteratorRWFile!$B$1:$N$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="13"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -3780,12 +4397,33 @@
                         <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="5">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
                         <c:v>16</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="9">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
                         <c:v>32</c:v>
                       </c:pt>
                     </c:numCache>
@@ -3793,7 +4431,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>iteratorRWFile!#REF!</c15:sqref>
@@ -3810,7 +4448,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-3D6A-4133-BA19-CBD7ACEBF3CA}"/>
                   </c:ext>
@@ -4200,7 +4838,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> - Read-Only Iteration (8-Core)</a:t>
+              <a:t> - Read-Only Iteration (24-Core)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4249,7 +4887,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ConcurrentMap (Interlocked)</c:v>
+                  <c:v>ConcurrentMap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4281,10 +4919,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>iteratorROFile!$B$1:$G$1</c:f>
+              <c:f>iteratorROFile!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4295,12 +4933,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -4308,27 +4967,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>iteratorROFile!$B$2:$G$2</c:f>
+              <c:f>iteratorROFile!$B$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>31.25</c:v>
+                  <c:v>23.26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.63</c:v>
+                  <c:v>29.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>90.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>142.86000000000001</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>142.86000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>125</c:v>
+                <c:pt idx="6">
+                  <c:v>166.67</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4379,10 +5059,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>iteratorROFile!$B$1:$G$1</c:f>
+              <c:f>iteratorROFile!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4393,12 +5073,33 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -4406,27 +5107,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>iteratorROFile!$B$3:$G$3</c:f>
+              <c:f>iteratorROFile!$B$3:$N$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>52.63</c:v>
+                  <c:v>41.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>111.11</c:v>
+                  <c:v>76.92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>166.67</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>250</c:v>
+                  <c:v>333.33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>250</c:v>
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4503,13 +5225,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>iteratorROFile!$B$1:$G$1</c15:sqref>
+                          <c15:sqref>iteratorROFile!$B$1:$N$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="13"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -4520,12 +5242,33 @@
                         <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="5">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
                         <c:v>16</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="9">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
                         <c:v>32</c:v>
                       </c:pt>
                     </c:numCache>
@@ -4553,13 +5296,13 @@
                         <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="4">
-                        <c:v>16</c:v>
-                      </c:pt>
                       <c:pt idx="5">
-                        <c:v>32</c:v>
+                        <c:v>10</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4578,7 +5321,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>iteratorROFile!#REF!</c15:sqref>
@@ -4623,13 +5366,13 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>iteratorROFile!$B$1:$G$1</c15:sqref>
+                          <c15:sqref>iteratorROFile!$B$1:$N$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="13"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -4640,12 +5383,33 @@
                         <c:v>4</c:v>
                       </c:pt>
                       <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
                         <c:v>8</c:v>
                       </c:pt>
-                      <c:pt idx="4">
+                      <c:pt idx="5">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
                         <c:v>16</c:v>
                       </c:pt>
-                      <c:pt idx="5">
+                      <c:pt idx="9">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
                         <c:v>32</c:v>
                       </c:pt>
                     </c:numCache>
@@ -4653,7 +5417,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>iteratorROFile!#REF!</c15:sqref>
@@ -4670,7 +5434,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-8208-4BBE-B712-F8E8258C3E2D}"/>
                   </c:ext>
@@ -7870,13 +8634,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>176211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7905,13 +8669,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>541020</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8301,15 +9065,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8323,82 +9087,166 @@
         <v>4</v>
       </c>
       <c r="E1">
+        <v>6</v>
+      </c>
+      <c r="F1">
         <v>8</v>
       </c>
-      <c r="F1">
+      <c r="G1">
+        <v>10</v>
+      </c>
+      <c r="H1">
+        <v>12</v>
+      </c>
+      <c r="I1">
+        <v>14</v>
+      </c>
+      <c r="J1">
         <v>16</v>
       </c>
-      <c r="G1">
+      <c r="K1">
+        <v>20</v>
+      </c>
+      <c r="L1">
+        <v>24</v>
+      </c>
+      <c r="M1">
+        <v>28</v>
+      </c>
+      <c r="N1">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3.7</v>
+        <v>2.99</v>
       </c>
       <c r="C2">
-        <v>7.19</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D2">
-        <v>13.33</v>
+        <v>8.4700000000000006</v>
       </c>
       <c r="E2">
-        <v>20.83</v>
+        <v>11.76</v>
       </c>
       <c r="F2">
-        <v>21.74</v>
+        <v>13.89</v>
       </c>
       <c r="G2">
-        <v>21.28</v>
+        <v>16.13</v>
+      </c>
+      <c r="H2">
+        <v>17.86</v>
+      </c>
+      <c r="I2">
+        <v>19.61</v>
+      </c>
+      <c r="J2">
+        <v>20.41</v>
+      </c>
+      <c r="K2">
+        <v>23.26</v>
+      </c>
+      <c r="L2">
+        <v>25.64</v>
+      </c>
+      <c r="M2">
+        <v>26.32</v>
+      </c>
+      <c r="N2">
+        <v>25.64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>6.33</v>
+      </c>
+      <c r="C3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D3">
+        <v>3.66</v>
+      </c>
+      <c r="E3">
+        <v>3.24</v>
+      </c>
+      <c r="F3">
+        <v>2.86</v>
+      </c>
+      <c r="G3">
+        <v>2.74</v>
+      </c>
+      <c r="H3">
+        <v>2.77</v>
+      </c>
+      <c r="I3">
+        <v>2.82</v>
+      </c>
+      <c r="J3">
+        <v>2.77</v>
+      </c>
+      <c r="K3">
+        <v>2.67</v>
+      </c>
+      <c r="L3">
+        <v>2.58</v>
+      </c>
+      <c r="M3">
+        <v>2.35</v>
+      </c>
+      <c r="N3">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>6.21</v>
-      </c>
-      <c r="C3">
+      <c r="B4">
         <v>5.71</v>
       </c>
-      <c r="D3">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="E3">
-        <v>4.07</v>
-      </c>
-      <c r="F3">
-        <v>4.12</v>
-      </c>
-      <c r="G3">
-        <v>4.1500000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>6.33</v>
-      </c>
       <c r="C4">
-        <v>3.91</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="D4">
-        <v>3.53</v>
+        <v>4.08</v>
       </c>
       <c r="E4">
-        <v>3.55</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>2.82</v>
+        <v>4.03</v>
       </c>
       <c r="G4">
-        <v>3.29</v>
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>4.03</v>
+      </c>
+      <c r="J4">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="K4">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -8409,17 +9257,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -8431,105 +9279,166 @@
         <v>4</v>
       </c>
       <c r="E1">
+        <v>6</v>
+      </c>
+      <c r="F1">
         <v>8</v>
       </c>
-      <c r="F1">
+      <c r="G1">
+        <v>10</v>
+      </c>
+      <c r="H1">
+        <v>12</v>
+      </c>
+      <c r="I1">
+        <v>14</v>
+      </c>
+      <c r="J1">
         <v>16</v>
       </c>
-      <c r="G1">
+      <c r="K1">
+        <v>20</v>
+      </c>
+      <c r="L1">
+        <v>24</v>
+      </c>
+      <c r="M1">
+        <v>28</v>
+      </c>
+      <c r="N1">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>21.28</v>
+        <v>13.16</v>
       </c>
       <c r="C2">
-        <v>34.479999999999997</v>
+        <v>17.86</v>
       </c>
       <c r="D2">
-        <v>66.67</v>
+        <v>35.71</v>
       </c>
       <c r="E2">
+        <v>55.56</v>
+      </c>
+      <c r="F2">
+        <v>76.92</v>
+      </c>
+      <c r="G2">
         <v>90.91</v>
       </c>
-      <c r="F2">
-        <v>90.91</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
+      <c r="H2">
+        <v>111.11</v>
+      </c>
+      <c r="I2">
+        <v>125</v>
+      </c>
+      <c r="J2">
+        <v>142.86000000000001</v>
+      </c>
+      <c r="K2">
+        <v>166.67</v>
+      </c>
+      <c r="L2">
+        <v>166.67</v>
+      </c>
+      <c r="M2">
+        <v>166.67</v>
+      </c>
+      <c r="N2">
+        <v>166.67</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>19.23</v>
+        <v>25.64</v>
       </c>
       <c r="C3">
-        <v>33.33</v>
+        <v>23.81</v>
       </c>
       <c r="D3">
-        <v>58.82</v>
+        <v>23.26</v>
       </c>
       <c r="E3">
-        <v>83.33</v>
+        <v>23.26</v>
       </c>
       <c r="F3">
-        <v>83.33</v>
+        <v>23.26</v>
       </c>
       <c r="G3">
-        <v>83.33</v>
+        <v>23.26</v>
+      </c>
+      <c r="H3">
+        <v>23.26</v>
+      </c>
+      <c r="I3">
+        <v>23.26</v>
+      </c>
+      <c r="J3">
+        <v>23.26</v>
+      </c>
+      <c r="K3">
+        <v>23.26</v>
+      </c>
+      <c r="L3">
+        <v>23.26</v>
+      </c>
+      <c r="M3">
+        <v>23.26</v>
+      </c>
+      <c r="N3">
+        <v>23.26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>32.26</v>
+        <v>25.64</v>
       </c>
       <c r="C4">
-        <v>27.78</v>
+        <v>19.61</v>
       </c>
       <c r="D4">
-        <v>27.78</v>
+        <v>20</v>
       </c>
       <c r="E4">
-        <v>27.78</v>
+        <v>20</v>
       </c>
       <c r="F4">
-        <v>27.78</v>
+        <v>20</v>
       </c>
       <c r="G4">
-        <v>27.78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>30.26</v>
-      </c>
-      <c r="C5">
-        <v>25.78</v>
-      </c>
-      <c r="D5">
-        <v>25.78</v>
-      </c>
-      <c r="E5">
-        <v>25.78</v>
-      </c>
-      <c r="F5">
-        <v>25.78</v>
-      </c>
-      <c r="G5">
-        <v>25.78</v>
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <v>20</v>
+      </c>
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+      <c r="N4">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -8540,17 +9449,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -8562,105 +9471,166 @@
         <v>4</v>
       </c>
       <c r="E1">
+        <v>6</v>
+      </c>
+      <c r="F1">
         <v>8</v>
       </c>
-      <c r="F1">
+      <c r="G1">
+        <v>10</v>
+      </c>
+      <c r="H1">
+        <v>12</v>
+      </c>
+      <c r="I1">
+        <v>14</v>
+      </c>
+      <c r="J1">
         <v>16</v>
       </c>
-      <c r="G1">
+      <c r="K1">
+        <v>20</v>
+      </c>
+      <c r="L1">
+        <v>24</v>
+      </c>
+      <c r="M1">
+        <v>28</v>
+      </c>
+      <c r="N1">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.92</v>
+        <v>7.35</v>
       </c>
       <c r="C2">
-        <v>3.21</v>
+        <v>10.1</v>
       </c>
       <c r="D2">
-        <v>6.17</v>
+        <v>22.73</v>
       </c>
       <c r="E2">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="F2">
+        <v>43.48</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>55.56</v>
+      </c>
+      <c r="I2">
+        <v>62.5</v>
+      </c>
+      <c r="J2">
+        <v>71.430000000000007</v>
+      </c>
+      <c r="K2">
+        <v>76.92</v>
+      </c>
+      <c r="L2">
+        <v>90.91</v>
+      </c>
+      <c r="M2">
+        <v>90.91</v>
+      </c>
+      <c r="N2">
+        <v>90.91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="C3">
+        <v>8.26</v>
+      </c>
+      <c r="D3">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="E3">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F2">
-        <v>8.06</v>
-      </c>
-      <c r="G2">
-        <v>7.94</v>
+      <c r="F3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="H3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J3">
+        <v>8.26</v>
+      </c>
+      <c r="K3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L3">
+        <v>8.26</v>
+      </c>
+      <c r="M3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N3">
+        <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="C3">
-        <v>18.87</v>
-      </c>
-      <c r="D3">
-        <v>29.41</v>
-      </c>
-      <c r="E3">
-        <v>45.45</v>
-      </c>
-      <c r="F3">
-        <v>45.45</v>
-      </c>
-      <c r="G3">
-        <v>47.62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>12.2</v>
+        <v>8.6199999999999992</v>
       </c>
       <c r="C4">
-        <v>11.9</v>
+        <v>8.4</v>
       </c>
       <c r="D4">
-        <v>11.63</v>
+        <v>8.26</v>
       </c>
       <c r="E4">
-        <v>11.76</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F4">
-        <v>11.63</v>
+        <v>8.26</v>
       </c>
       <c r="G4">
-        <v>11.76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>12.35</v>
-      </c>
-      <c r="C5">
-        <v>11.76</v>
-      </c>
-      <c r="D5">
-        <v>11.49</v>
-      </c>
-      <c r="E5">
-        <v>11.76</v>
-      </c>
-      <c r="F5">
-        <v>11.9</v>
-      </c>
-      <c r="G5">
-        <v>11.9</v>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="H4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I4">
+        <v>8.26</v>
+      </c>
+      <c r="J4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K4">
+        <v>8.26</v>
+      </c>
+      <c r="L4">
+        <v>8.26</v>
+      </c>
+      <c r="M4">
+        <v>8.26</v>
+      </c>
+      <c r="N4">
+        <v>8.26</v>
       </c>
     </row>
   </sheetData>
@@ -8671,17 +9641,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -8693,82 +9663,166 @@
         <v>4</v>
       </c>
       <c r="E1">
+        <v>6</v>
+      </c>
+      <c r="F1">
         <v>8</v>
       </c>
-      <c r="F1">
+      <c r="G1">
+        <v>10</v>
+      </c>
+      <c r="H1">
+        <v>12</v>
+      </c>
+      <c r="I1">
+        <v>14</v>
+      </c>
+      <c r="J1">
         <v>16</v>
       </c>
-      <c r="G1">
+      <c r="K1">
+        <v>20</v>
+      </c>
+      <c r="L1">
+        <v>24</v>
+      </c>
+      <c r="M1">
+        <v>28</v>
+      </c>
+      <c r="N1">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>16.13</v>
+        <v>11.63</v>
       </c>
       <c r="C2">
-        <v>27.78</v>
+        <v>16.39</v>
       </c>
       <c r="D2">
+        <v>33.33</v>
+      </c>
+      <c r="E2">
         <v>50</v>
-      </c>
-      <c r="E2">
-        <v>71.430000000000007</v>
       </c>
       <c r="F2">
         <v>66.67</v>
       </c>
       <c r="G2">
-        <v>66.67</v>
+        <v>83.33</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>111.11</v>
+      </c>
+      <c r="J2">
+        <v>111.11</v>
+      </c>
+      <c r="K2">
+        <v>125</v>
+      </c>
+      <c r="L2">
+        <v>142.86000000000001</v>
+      </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
+      <c r="N2">
+        <v>90.91</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C3">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="D3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="E3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="F3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="G3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="H3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="I3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="J3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="K3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="L3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="M3">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="N3">
+        <v>9.7100000000000009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>18.52</v>
-      </c>
-      <c r="C3">
-        <v>17.86</v>
-      </c>
-      <c r="D3">
-        <v>17.54</v>
-      </c>
-      <c r="E3">
-        <v>17.54</v>
-      </c>
-      <c r="F3">
-        <v>17.54</v>
-      </c>
-      <c r="G3">
-        <v>17.54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
       <c r="B4">
-        <v>18.52</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C4">
-        <v>17.54</v>
+        <v>9.7100000000000009</v>
       </c>
       <c r="D4">
-        <v>17.239999999999998</v>
+        <v>9.6199999999999992</v>
       </c>
       <c r="E4">
-        <v>17.239999999999998</v>
+        <v>9.6199999999999992</v>
       </c>
       <c r="F4">
-        <v>17.239999999999998</v>
+        <v>9.6199999999999992</v>
       </c>
       <c r="G4">
-        <v>17.239999999999998</v>
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="H4">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="I4">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="J4">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="K4">
+        <v>9.52</v>
+      </c>
+      <c r="L4">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="M4">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="N4">
+        <v>9.6199999999999992</v>
       </c>
     </row>
   </sheetData>
@@ -8779,17 +9833,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -8801,59 +9855,122 @@
         <v>4</v>
       </c>
       <c r="E1">
+        <v>6</v>
+      </c>
+      <c r="F1">
         <v>8</v>
       </c>
-      <c r="F1">
+      <c r="G1">
+        <v>10</v>
+      </c>
+      <c r="H1">
+        <v>12</v>
+      </c>
+      <c r="I1">
+        <v>14</v>
+      </c>
+      <c r="J1">
         <v>16</v>
       </c>
-      <c r="G1">
+      <c r="K1">
+        <v>20</v>
+      </c>
+      <c r="L1">
+        <v>24</v>
+      </c>
+      <c r="M1">
+        <v>28</v>
+      </c>
+      <c r="N1">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>31.25</v>
+        <v>23.26</v>
       </c>
       <c r="C2">
-        <v>52.63</v>
+        <v>29.41</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>62.5</v>
       </c>
       <c r="E2">
+        <v>90.91</v>
+      </c>
+      <c r="F2">
+        <v>125</v>
+      </c>
+      <c r="G2">
         <v>142.86000000000001</v>
       </c>
-      <c r="F2">
-        <v>142.86000000000001</v>
-      </c>
-      <c r="G2">
-        <v>125</v>
+      <c r="H2">
+        <v>166.67</v>
+      </c>
+      <c r="I2">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>200</v>
+      </c>
+      <c r="K2">
+        <v>250</v>
+      </c>
+      <c r="L2">
+        <v>250</v>
+      </c>
+      <c r="M2">
+        <v>250</v>
+      </c>
+      <c r="N2">
+        <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>52.63</v>
+        <v>41.67</v>
       </c>
       <c r="C3">
-        <v>111.11</v>
+        <v>76.92</v>
       </c>
       <c r="D3">
-        <v>200</v>
+        <v>166.67</v>
       </c>
       <c r="E3">
         <v>250</v>
       </c>
       <c r="F3">
-        <v>250</v>
+        <v>333.33</v>
       </c>
       <c r="G3">
-        <v>250</v>
+        <v>500</v>
+      </c>
+      <c r="H3">
+        <v>500</v>
+      </c>
+      <c r="I3">
+        <v>500</v>
+      </c>
+      <c r="J3">
+        <v>500</v>
+      </c>
+      <c r="K3">
+        <v>500</v>
+      </c>
+      <c r="L3">
+        <v>1000</v>
+      </c>
+      <c r="M3">
+        <v>1000</v>
+      </c>
+      <c r="N3">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated README to demonstrate changes I made to Go. As well, I made it so the iterator does not bother spinning at all (or yielding) when it finds a locked bucket, but merely adds it to it's list of skipped buckets.
</commit_message>
<xml_diff>
--- a/map_testing/benchmark.xlsx
+++ b/map_testing/benchmark.xlsx
@@ -2230,7 +2230,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>combinedFile!#REF!</c15:sqref>
@@ -2272,7 +2272,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>combinedFile!$B$1:$N$1</c15:sqref>
@@ -2326,7 +2326,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>combinedFile!#REF!</c15:sqref>
@@ -2343,7 +2343,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-BE45-4C25-A0FE-13F21B9F3CEF}"/>
                   </c:ext>
@@ -4377,7 +4377,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>iteratorRWFile!$B$1:$N$1</c15:sqref>
@@ -5363,7 +5363,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>iteratorROFile!$B$1:$N$1</c15:sqref>
@@ -8765,6 +8765,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>342357</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>134520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13411200" y="2743200"/>
+          <a:ext cx="11315157" cy="4706520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9836,7 +9874,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>